<commit_message>
aiinthewild Lab 5 init
</commit_message>
<xml_diff>
--- a/AI_In_Wild/Lab4/absExample-lab.xlsx
+++ b/AI_In_Wild/Lab4/absExample-lab.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gameuser\Desktop\Year_4\AI_In_Wild\Lab4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D17B970-22D1-4ADA-8FD1-243CF35C8F6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902D9222-E234-4E27-8B12-1F5995274ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{56DC7B23-590F-4E30-B993-F1A4F72C03A3}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
   <si>
     <t>B</t>
   </si>
@@ -144,12 +144,15 @@
   <si>
     <t>A Protect Behaviour</t>
   </si>
+  <si>
+    <t>C2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +194,21 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -240,7 +258,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -307,6 +325,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -440,30 +464,30 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F517C5CC-2B4E-4931-8651-A1B53D0D1B36}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{9C11CDA7-CCEA-4509-8745-17D00E9FEF5B}" type="CELLRANGE">
+                      <a:rPr lang="en-IE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
                     <a:r>
-                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:rPr lang="en-IE" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{9DF1C46E-D4AF-4DD8-A3C2-9CD93B0545A7}" type="XVALUE">
-                      <a:rPr lang="en-US" baseline="0"/>
+                    <a:fld id="{1DF33408-C818-45CF-9F47-C78ECCAA0D3A}" type="XVALUE">
+                      <a:rPr lang="en-IE" baseline="0"/>
                       <a:pPr/>
                       <a:t>[X VALUE]</a:t>
                     </a:fld>
                     <a:r>
-                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:rPr lang="en-IE" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{C8D172DF-3C48-4117-992A-EE76091DC9FE}" type="YVALUE">
-                      <a:rPr lang="en-US" baseline="0"/>
+                    <a:fld id="{20067870-932A-43EA-92B3-FFD74444F191}" type="YVALUE">
+                      <a:rPr lang="en-IE" baseline="0"/>
                       <a:pPr/>
                       <a:t>[Y VALUE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US" baseline="0"/>
+                    <a:endParaRPr lang="en-IE" baseline="0"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -492,30 +516,30 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2961BF55-83A9-4A20-8628-C17A5A04FF4F}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{8CF260C0-56C1-4B6C-82DB-4993C81DD5A8}" type="CELLRANGE">
+                      <a:rPr lang="en-IE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
                     <a:r>
-                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:rPr lang="en-IE" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{13C331F2-4D7A-4B63-8367-42A246BEE116}" type="XVALUE">
-                      <a:rPr lang="en-US" baseline="0"/>
+                    <a:fld id="{1DFA4C49-C263-49F7-BDC2-9F7EA7F38B6A}" type="XVALUE">
+                      <a:rPr lang="en-IE" baseline="0"/>
                       <a:pPr/>
                       <a:t>[X VALUE]</a:t>
                     </a:fld>
                     <a:r>
-                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:rPr lang="en-IE" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{EA86F726-55EF-48DE-9A73-47E10DE92610}" type="YVALUE">
-                      <a:rPr lang="en-US" baseline="0"/>
+                    <a:fld id="{17C03A98-6E24-4DD8-815B-D8BEB62E395A}" type="YVALUE">
+                      <a:rPr lang="en-IE" baseline="0"/>
                       <a:pPr/>
                       <a:t>[Y VALUE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US" baseline="0"/>
+                    <a:endParaRPr lang="en-IE" baseline="0"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -544,30 +568,30 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AF6815BD-B939-409F-869E-03AF5581B8FA}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{82B01926-38E8-4272-9D03-06E9DCBE1D24}" type="CELLRANGE">
+                      <a:rPr lang="en-IE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
                     <a:r>
-                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:rPr lang="en-IE" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{5F0EDE96-2953-4B62-A98B-CE32EC66F77E}" type="XVALUE">
-                      <a:rPr lang="en-US" baseline="0"/>
+                    <a:fld id="{CC7070EB-B3DA-4F86-BFA3-0D65E3AA2A1F}" type="XVALUE">
+                      <a:rPr lang="en-IE" baseline="0"/>
                       <a:pPr/>
                       <a:t>[X VALUE]</a:t>
                     </a:fld>
                     <a:r>
-                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:rPr lang="en-IE" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{81E08D4A-22C0-4EFB-949E-D49CEC28571F}" type="YVALUE">
-                      <a:rPr lang="en-US" baseline="0"/>
+                    <a:fld id="{61A24119-264D-4648-8868-3B6263E6F044}" type="YVALUE">
+                      <a:rPr lang="en-IE" baseline="0"/>
                       <a:pPr/>
                       <a:t>[Y VALUE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US" baseline="0"/>
+                    <a:endParaRPr lang="en-IE" baseline="0"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -596,30 +620,30 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9269F728-DD32-4771-A252-403446A84239}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{467234DE-D9BB-47C4-AF77-2C7FA8333D9D}" type="CELLRANGE">
+                      <a:rPr lang="en-IE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
                     <a:r>
-                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:rPr lang="en-IE" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{EE685129-8683-446B-A6BA-6ABCC81AD7CF}" type="XVALUE">
-                      <a:rPr lang="en-US" baseline="0"/>
+                    <a:fld id="{87745C51-320B-412E-90A6-D2C8957FCAF9}" type="XVALUE">
+                      <a:rPr lang="en-IE" baseline="0"/>
                       <a:pPr/>
                       <a:t>[X VALUE]</a:t>
                     </a:fld>
                     <a:r>
-                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:rPr lang="en-IE" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{DF47E409-BFB9-47BD-879B-67DFB96A4139}" type="YVALUE">
-                      <a:rPr lang="en-US" baseline="0"/>
+                    <a:fld id="{EA24E46D-FF4F-440A-9BF7-57D835D517FF}" type="YVALUE">
+                      <a:rPr lang="en-IE" baseline="0"/>
                       <a:pPr/>
                       <a:t>[Y VALUE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US" baseline="0"/>
+                    <a:endParaRPr lang="en-IE" baseline="0"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1108,7 +1132,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{40F6228E-81B7-4D71-983D-9E1C0C3B0818}" type="CELLRANGE">
+                    <a:fld id="{29AE48CD-F3E3-4E1A-902C-21524B69971E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1117,7 +1141,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{DCE6C00C-EE33-492D-BD4A-A7D56C4D1E60}" type="XVALUE">
+                    <a:fld id="{29DA8849-5376-4F09-A3B1-8193E43A91DA}" type="XVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[X VALUE]</a:t>
@@ -1126,7 +1150,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{1CD6B55A-19AD-4964-B76A-47D1582892F8}" type="YVALUE">
+                    <a:fld id="{731BEC43-6AEC-4C22-BCBB-B95FFBB22D79}" type="YVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[Y VALUE]</a:t>
@@ -1160,7 +1184,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{10A45EC0-53ED-403D-898F-73E26B867C7E}" type="CELLRANGE">
+                    <a:fld id="{928A9B42-6048-4803-8F41-A2577A9DB60E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1169,7 +1193,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{A8D3E1FD-7B05-4FDB-881A-FC8330AE2FB2}" type="XVALUE">
+                    <a:fld id="{78DD6A06-9A9D-4023-9BBD-33D6E208D058}" type="XVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[X VALUE]</a:t>
@@ -1178,7 +1202,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{8CDDDB4F-4AFA-491D-A651-BCFAA53D8B53}" type="YVALUE">
+                    <a:fld id="{836CE070-C1A1-43E0-ADCA-45F1F452F1D6}" type="YVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[Y VALUE]</a:t>
@@ -1212,7 +1236,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FCBA5257-8114-4929-B113-C2BADED805C1}" type="CELLRANGE">
+                    <a:fld id="{1F83551B-77EE-44EE-8A2D-A31B6A82F55F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1221,7 +1245,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{C7743A9D-A9A0-4013-8B64-9B78B91A2F80}" type="XVALUE">
+                    <a:fld id="{26B565AF-0F27-49EF-BD46-EF29C298B353}" type="XVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[X VALUE]</a:t>
@@ -1230,7 +1254,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{E99AEF75-0238-4D61-9785-6F15242139BF}" type="YVALUE">
+                    <a:fld id="{A0729B88-0F35-4627-8D6B-8DCCFC69A4AC}" type="YVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[Y VALUE]</a:t>
@@ -1264,7 +1288,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9BF5037B-E30C-482C-BFEF-9DDB3B421317}" type="CELLRANGE">
+                    <a:fld id="{AA423E40-10DF-4D84-9D71-4E1D1F5D186B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1273,7 +1297,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{FF34943C-5EA8-4DFB-9EC2-889A809DE02A}" type="XVALUE">
+                    <a:fld id="{732B31E3-03B9-4071-A3DE-BB76FC2254A1}" type="XVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[X VALUE]</a:t>
@@ -1282,7 +1306,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{A7866885-D101-4DB2-91A9-AB72B5DC2E7A}" type="YVALUE">
+                    <a:fld id="{316F8814-C725-4D5E-A9EE-A34483E1E3C7}" type="YVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[Y VALUE]</a:t>
@@ -1316,7 +1340,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8C85BE64-4FC2-4400-8682-A4423E52DCAD}" type="CELLRANGE">
+                    <a:fld id="{1790FBC0-FE9B-4F01-86CF-8DF9B9C4E02E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1325,7 +1349,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{C7D51612-1AFC-4D34-8B2C-3A01B0E5A96D}" type="XVALUE">
+                    <a:fld id="{33AEF4F1-4CBF-4F19-90AB-485757CCC735}" type="XVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[X VALUE]</a:t>
@@ -1334,7 +1358,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>, </a:t>
                     </a:r>
-                    <a:fld id="{7411AB68-0BAC-4214-A0AB-30A1512BEB95}" type="YVALUE">
+                    <a:fld id="{A1DB8D59-83F2-4748-B0FF-E413DD99782E}" type="YVALUE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[Y VALUE]</a:t>
@@ -3466,7 +3490,7 @@
   <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3658,9 +3682,17 @@
         <f>L14/K15</f>
         <v>0.51449575542752646</v>
       </c>
-      <c r="N16" s="9"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
+      <c r="N16" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="O16" s="25">
+        <f>K19</f>
+        <v>0</v>
+      </c>
+      <c r="P16" s="25">
+        <f>L19</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I17" s="4" t="s">
@@ -3696,6 +3728,9 @@
       <c r="P18" s="16"/>
     </row>
     <row r="19" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="J19" s="21" t="s">
+        <v>36</v>
+      </c>
       <c r="M19" s="1"/>
       <c r="N19" s="9"/>
       <c r="O19" s="10"/>

</xml_diff>